<commit_message>
puzzle day 2 + a zillion claimed puzzles
</commit_message>
<xml_diff>
--- a/constructors.xlsx
+++ b/constructors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="75">
   <si>
     <t>Jan</t>
   </si>
@@ -204,6 +204,51 @@
   </si>
   <si>
     <t>CHARLOTTE DEMING</t>
+  </si>
+  <si>
+    <t>WILL EISENBERG</t>
+  </si>
+  <si>
+    <t>SOPHIA MAYMUDES</t>
+  </si>
+  <si>
+    <t>SOPHIA MAYAMUDES</t>
+  </si>
+  <si>
+    <t>DEREK ALLEN</t>
+  </si>
+  <si>
+    <t>TOM TABANAO</t>
+  </si>
+  <si>
+    <t>lyle / jack</t>
+  </si>
+  <si>
+    <t>DOUG PETERSON</t>
+  </si>
+  <si>
+    <t>KEN STERN</t>
+  </si>
+  <si>
+    <t>MICHAEL LIEBERMAN</t>
+  </si>
+  <si>
+    <t>SAL DADDARIO</t>
+  </si>
+  <si>
+    <t>JONATHAN KAYE</t>
+  </si>
+  <si>
+    <t>ELLEN ZEMLIN</t>
+  </si>
+  <si>
+    <t>SAM BUCHBINDER</t>
+  </si>
+  <si>
+    <t>ARDIAN POWELL</t>
+  </si>
+  <si>
+    <t>JAC CRABTREE</t>
   </si>
 </sst>
 </file>
@@ -219,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,7 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -360,6 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,8 +751,8 @@
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
@@ -747,7 +798,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="18"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
@@ -775,11 +826,11 @@
       <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -806,7 +857,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="9" t="s">
         <v>45</v>
       </c>
@@ -823,10 +874,10 @@
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="O5" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="P5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R5" t="s">
         <v>32</v>
@@ -842,14 +893,16 @@
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="18"/>
+      <c r="H6" s="17"/>
       <c r="I6" s="7"/>
       <c r="J6" s="9" t="s">
         <v>35</v>
@@ -858,10 +911,10 @@
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
       <c r="O6" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R6" t="s">
         <v>13</v>
@@ -877,7 +930,9 @@
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="D7" s="9" t="s">
         <v>23</v>
       </c>
@@ -886,12 +941,12 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="8"/>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="P7">
         <v>1</v>
@@ -916,7 +971,7 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="18"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -924,13 +979,13 @@
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
       <c r="O8" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="P8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -943,8 +998,8 @@
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
@@ -959,13 +1014,13 @@
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
       <c r="O9" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="P9">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="S9">
         <v>1</v>
@@ -992,22 +1047,22 @@
         <v>36</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
       <c r="O10" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="S10">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -1026,7 +1081,7 @@
       <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1035,13 +1090,13 @@
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
       <c r="O11" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="S11">
         <v>1</v>
@@ -1051,8 +1106,10 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1064,16 +1121,16 @@
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="O12" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="P12">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R12" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="S12">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1083,16 +1140,16 @@
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="6" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="17"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="18"/>
+      <c r="H13" s="17"/>
       <c r="I13" s="7"/>
       <c r="J13" s="9" t="s">
         <v>38</v>
@@ -1101,13 +1158,13 @@
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
       <c r="O13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="S13">
         <v>1</v>
@@ -1131,18 +1188,18 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
       <c r="O14" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="P14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="S14">
         <v>1</v>
@@ -1161,30 +1218,32 @@
       <c r="D15" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="F15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="11" t="s">
         <v>26</v>
       </c>
       <c r="O15" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="P15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R15" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="S15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -1194,8 +1253,8 @@
       <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -1210,16 +1269,16 @@
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
       <c r="O16" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>17</v>
+      </c>
+      <c r="S16">
         <v>2</v>
-      </c>
-      <c r="R16" t="s">
-        <v>53</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
@@ -1229,7 +1288,9 @@
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="D17" s="6" t="s">
         <v>52</v>
       </c>
@@ -1241,7 +1302,7 @@
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="6" t="s">
         <v>52</v>
       </c>
@@ -1249,13 +1310,13 @@
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
       <c r="O17" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="P17">
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="S17">
         <v>1</v>
@@ -1275,7 +1336,7 @@
         <v>55</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="18"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="7"/>
       <c r="H18" s="9" t="s">
         <v>49</v>
@@ -1284,17 +1345,17 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="12" t="s">
+      <c r="M18" s="11" t="s">
         <v>32</v>
       </c>
       <c r="O18" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R18" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -1304,7 +1365,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="20"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="9" t="s">
         <v>32</v>
       </c>
@@ -1322,15 +1383,17 @@
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
+      <c r="O19" t="s">
+        <v>37</v>
+      </c>
       <c r="P19">
-        <f>SUM(P2:P18)</f>
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="R19" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="S19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
@@ -1346,20 +1409,26 @@
       <c r="D20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="18"/>
+      <c r="H20" s="17"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="8"/>
+      <c r="O20" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
       <c r="R20" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="S20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
@@ -1369,7 +1438,9 @@
       <c r="B21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="D21" s="7"/>
       <c r="E21" s="9" t="s">
         <v>33</v>
@@ -1380,12 +1451,18 @@
         <v>47</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="17"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
+      <c r="O21" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
       <c r="R21" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="S21">
         <v>1</v>
@@ -1398,22 +1475,34 @@
       <c r="B22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="18"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
+      <c r="O22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
       <c r="R22" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="S22">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
@@ -1423,8 +1512,8 @@
       <c r="B23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1436,8 +1525,12 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="8"/>
+      <c r="P23">
+        <f>SUM(P2:P22)</f>
+        <v>48</v>
+      </c>
       <c r="R23" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="S23">
         <v>1</v>
@@ -1458,16 +1551,16 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="8"/>
       <c r="R24" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="S24">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
@@ -1482,20 +1575,22 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="18"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="J25" s="7"/>
       <c r="K25" s="9" t="s">
         <v>34</v>
       </c>
       <c r="L25" s="7"/>
-      <c r="M25" s="12" t="s">
+      <c r="M25" s="11" t="s">
         <v>26</v>
       </c>
       <c r="R25" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="S25">
         <v>1</v>
@@ -1505,8 +1600,10 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="D26" s="7"/>
       <c r="E26" s="9" t="s">
         <v>32</v>
@@ -1515,17 +1612,21 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
+      <c r="J26" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="13" t="s">
+      <c r="L26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M26" s="12" t="s">
         <v>16</v>
       </c>
       <c r="R26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S26">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
@@ -1535,21 +1636,23 @@
       <c r="B27" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="18"/>
+      <c r="E27" s="17"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="18"/>
+      <c r="H27" s="17"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="8"/>
       <c r="R27" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="S27">
         <v>1</v>
@@ -1562,8 +1665,12 @@
       <c r="B28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+      <c r="C28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E28" s="6" t="s">
         <v>18</v>
       </c>
@@ -1572,18 +1679,20 @@
         <v>33</v>
       </c>
       <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
+      <c r="I28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="17"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="13" t="s">
+      <c r="M28" s="12" t="s">
         <v>18</v>
       </c>
       <c r="R28" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="S28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
@@ -1593,26 +1702,30 @@
       <c r="B29" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="D29" s="7"/>
       <c r="E29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="18"/>
+      <c r="F29" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="17"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
-      <c r="M29" s="12" t="s">
+      <c r="M29" s="11" t="s">
         <v>36</v>
       </c>
       <c r="R29" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="S29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
@@ -1622,8 +1735,8 @@
       <c r="B30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="9" t="s">
@@ -1636,12 +1749,14 @@
         <v>39</v>
       </c>
       <c r="L30" s="7"/>
-      <c r="M30" s="12" t="s">
+      <c r="M30" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="R30" t="s">
+        <v>33</v>
+      </c>
       <c r="S30">
-        <f>SUM(S2:S29)</f>
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
@@ -1651,40 +1766,120 @@
       <c r="B31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="G31" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="7"/>
-      <c r="M31" s="12" t="s">
+      <c r="M31" s="11" t="s">
         <v>33</v>
+      </c>
+      <c r="R31" t="s">
+        <v>42</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="16" t="s">
+      <c r="C32" s="18"/>
+      <c r="D32" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="16"/>
+      <c r="R32" t="s">
+        <v>69</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R33" t="s">
+        <v>72</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R34" t="s">
+        <v>26</v>
+      </c>
+      <c r="S34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R35" t="s">
+        <v>35</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R36" t="s">
+        <v>24</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R37" t="s">
+        <v>64</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R38" t="s">
+        <v>60</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R39" t="s">
+        <v>14</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="S40">
+        <f>SUM(S2:S39)</f>
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new why page, new constructors
</commit_message>
<xml_diff>
--- a/constructors.xlsx
+++ b/constructors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="86">
   <si>
     <t>Jan</t>
   </si>
@@ -221,9 +221,6 @@
     <t>TOM TABANAO</t>
   </si>
   <si>
-    <t>lyle / jack</t>
-  </si>
-  <si>
     <t>DOUG PETERSON</t>
   </si>
   <si>
@@ -249,6 +246,42 @@
   </si>
   <si>
     <t>JAC CRABTREE</t>
+  </si>
+  <si>
+    <t>KYRALEESE</t>
+  </si>
+  <si>
+    <t>KATJA BRINCK</t>
+  </si>
+  <si>
+    <t>EMMA FREEMAN</t>
+  </si>
+  <si>
+    <t>SALLY HOELSCHER</t>
+  </si>
+  <si>
+    <t>LYLE BROUGHTON</t>
+  </si>
+  <si>
+    <t>DAVID MILLER</t>
+  </si>
+  <si>
+    <t>ALLEGRA</t>
+  </si>
+  <si>
+    <t>MADDIE WALTER</t>
+  </si>
+  <si>
+    <t>REBECCA GOLDSTEIN</t>
+  </si>
+  <si>
+    <t>LAWRENCE DENES</t>
+  </si>
+  <si>
+    <t>NICHOLAS PAPPAS</t>
+  </si>
+  <si>
+    <t>PAO ROY</t>
   </si>
 </sst>
 </file>
@@ -264,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -286,12 +319,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -410,7 +437,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -804,7 +830,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
       <c r="O3" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -833,7 +859,9 @@
       <c r="F4" s="17"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="6" t="s">
@@ -841,7 +869,7 @@
       </c>
       <c r="M4" s="8"/>
       <c r="O4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -861,8 +889,12 @@
       <c r="C5" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -874,7 +906,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="O5" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -900,8 +932,12 @@
         <v>31</v>
       </c>
       <c r="E6" s="17"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="H6" s="17"/>
       <c r="I6" s="7"/>
       <c r="J6" s="9" t="s">
@@ -911,10 +947,10 @@
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
       <c r="O6" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R6" t="s">
         <v>13</v>
@@ -931,7 +967,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>23</v>
@@ -946,10 +982,10 @@
       <c r="L7" s="7"/>
       <c r="M7" s="8"/>
       <c r="O7" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R7" t="s">
         <v>38</v>
@@ -968,7 +1004,9 @@
       <c r="C8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="17"/>
@@ -979,13 +1017,13 @@
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
       <c r="O8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="P8">
         <v>1</v>
       </c>
       <c r="R8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -1014,13 +1052,13 @@
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
       <c r="O9" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="S9">
         <v>1</v>
@@ -1036,7 +1074,9 @@
       <c r="C10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>25</v>
       </c>
@@ -1046,20 +1086,22 @@
       <c r="G10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="I10" s="17"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="P10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="S10">
         <v>1</v>
@@ -1083,20 +1125,22 @@
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
       <c r="O11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="S11">
         <v>1</v>
@@ -1107,11 +1151,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="19"/>
-      <c r="C12" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="C12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1121,16 +1169,16 @@
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="O12" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="P12">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="R12" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="S12">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1150,7 +1198,9 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="7"/>
+      <c r="I13" s="7" t="s">
+        <v>83</v>
+      </c>
       <c r="J13" s="9" t="s">
         <v>38</v>
       </c>
@@ -1158,16 +1208,16 @@
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
       <c r="O13" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -1193,13 +1243,13 @@
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
       <c r="O14" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="S14">
         <v>1</v>
@@ -1234,13 +1284,13 @@
         <v>26</v>
       </c>
       <c r="O15" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="P15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="S15">
         <v>1</v>
@@ -1269,16 +1319,16 @@
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
       <c r="O16" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="S16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
@@ -1310,16 +1360,16 @@
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
       <c r="O17" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="P17">
+        <v>13</v>
+      </c>
+      <c r="R17" t="s">
+        <v>17</v>
+      </c>
+      <c r="S17">
         <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>67</v>
-      </c>
-      <c r="S17">
-        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
@@ -1349,13 +1399,13 @@
         <v>32</v>
       </c>
       <c r="O18" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="P18">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -1369,7 +1419,9 @@
       <c r="C19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1384,13 +1436,13 @@
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
       <c r="O19" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="P19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="S19">
         <v>1</v>
@@ -1419,13 +1471,13 @@
       <c r="L20" s="7"/>
       <c r="M20" s="8"/>
       <c r="O20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="P20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R20" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="S20">
         <v>2</v>
@@ -1439,30 +1491,36 @@
         <v>39</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="E21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="G21" s="7"/>
       <c r="H21" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="J21" s="17"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
       <c r="O21" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="P21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="S21">
         <v>1</v>
@@ -1486,20 +1544,20 @@
       <c r="G22" s="17"/>
       <c r="H22" s="7"/>
       <c r="I22" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
       <c r="O22" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="P22">
         <v>1</v>
       </c>
       <c r="R22" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="S22">
         <v>1</v>
@@ -1525,15 +1583,17 @@
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="8"/>
+      <c r="O23" t="s">
+        <v>44</v>
+      </c>
       <c r="P23">
-        <f>SUM(P2:P22)</f>
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="R23" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="S23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -1547,7 +1607,9 @@
         <v>14</v>
       </c>
       <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
@@ -1556,11 +1618,17 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="8"/>
+      <c r="O24" t="s">
+        <v>82</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
       <c r="R24" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="S24">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
@@ -1589,8 +1657,14 @@
       <c r="M25" s="11" t="s">
         <v>26</v>
       </c>
+      <c r="O25" t="s">
+        <v>18</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
       <c r="R25" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="S25">
         <v>1</v>
@@ -1602,9 +1676,11 @@
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="E26" s="9" t="s">
         <v>32</v>
       </c>
@@ -1617,16 +1693,22 @@
       </c>
       <c r="K26" s="7"/>
       <c r="L26" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M26" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="O26" t="s">
+        <v>77</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
       <c r="R26" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="S26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
@@ -1637,7 +1719,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>57</v>
@@ -1651,11 +1733,17 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="8"/>
+      <c r="O27" t="s">
+        <v>37</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
       <c r="R27" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="S27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
@@ -1688,11 +1776,17 @@
       <c r="M28" s="12" t="s">
         <v>18</v>
       </c>
+      <c r="O28" t="s">
+        <v>55</v>
+      </c>
+      <c r="P28">
+        <v>2</v>
+      </c>
       <c r="R28" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="S28">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
@@ -1703,29 +1797,37 @@
         <v>25</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="6" t="s">
         <v>55</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
+      <c r="J29" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="11" t="s">
         <v>36</v>
       </c>
+      <c r="O29" t="s">
+        <v>61</v>
+      </c>
+      <c r="P29">
+        <v>3</v>
+      </c>
       <c r="R29" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="S29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
@@ -1752,11 +1854,17 @@
       <c r="M30" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="O30" t="s">
+        <v>56</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
       <c r="R30" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="S30">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
@@ -1775,7 +1883,7 @@
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="17"/>
@@ -1785,11 +1893,15 @@
       <c r="M31" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="P31">
+        <f>SUM(P2:P30)</f>
+        <v>62</v>
+      </c>
       <c r="R31" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="S31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1813,7 +1925,7 @@
       <c r="L32" s="18"/>
       <c r="M32" s="16"/>
       <c r="R32" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="S32">
         <v>1</v>
@@ -1821,7 +1933,7 @@
     </row>
     <row r="33" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R33" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="S33">
         <v>1</v>
@@ -1829,15 +1941,15 @@
     </row>
     <row r="34" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R34" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="S34">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R35" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="S35">
         <v>1</v>
@@ -1845,7 +1957,7 @@
     </row>
     <row r="36" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R36" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="S36">
         <v>1</v>
@@ -1853,7 +1965,7 @@
     </row>
     <row r="37" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R37" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="S37">
         <v>1</v>
@@ -1861,24 +1973,56 @@
     </row>
     <row r="38" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R38" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="S38">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R39" t="s">
+        <v>35</v>
+      </c>
+      <c r="S39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R40" t="s">
+        <v>24</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R41" t="s">
+        <v>64</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R42" t="s">
+        <v>60</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R43" t="s">
         <v>14</v>
       </c>
-      <c r="S39">
+      <c r="S43">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="18:19" x14ac:dyDescent="0.35">
-      <c r="S40">
-        <f>SUM(S2:S39)</f>
-        <v>62</v>
+    <row r="44" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="S44">
+        <f>SUM(S2:S43)</f>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix text crowding on large screens by forcign 13 cols
</commit_message>
<xml_diff>
--- a/constructors.xlsx
+++ b/constructors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="106">
   <si>
     <t>Jan</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>ALICIA HUGGETT</t>
+  </si>
+  <si>
+    <t>MALAIKA HANDA</t>
   </si>
 </sst>
 </file>
@@ -778,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,7 +1363,9 @@
         <v>27</v>
       </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -1610,7 +1615,7 @@
         <v>12</v>
       </c>
       <c r="P21">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R21" t="s">
         <v>69</v>
@@ -2117,7 +2122,7 @@
     <row r="37" spans="15:19" x14ac:dyDescent="0.35">
       <c r="P37">
         <f>SUM(P2:P36)</f>
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R37" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
add more mali puzzles
</commit_message>
<xml_diff>
--- a/constructors.xlsx
+++ b/constructors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="115">
   <si>
     <t>Jan</t>
   </si>
@@ -384,7 +384,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +406,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,13 +525,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -866,8 +872,8 @@
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="3" t="s">
         <v>30</v>
       </c>
@@ -878,10 +884,10 @@
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="16"/>
       <c r="M2" s="4" t="s">
         <v>37</v>
       </c>
@@ -919,7 +925,7 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="17"/>
+      <c r="I3" s="16"/>
       <c r="J3" s="7"/>
       <c r="K3" s="9" t="s">
         <v>93</v>
@@ -957,7 +963,7 @@
       <c r="E4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
@@ -986,7 +992,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="9" t="s">
         <v>45</v>
       </c>
@@ -996,7 +1002,9 @@
       <c r="E5" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G5" s="9" t="s">
         <v>106</v>
       </c>
@@ -1005,7 +1013,7 @@
       <c r="J5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="7"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="O5" t="s">
@@ -1034,14 +1042,14 @@
       <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="6" t="s">
         <v>74</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="7"/>
       <c r="J6" s="9" t="s">
         <v>35</v>
@@ -1086,10 +1094,10 @@
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="16"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="8"/>
+      <c r="M7" s="16"/>
       <c r="O7" t="s">
         <v>71</v>
       </c>
@@ -1120,7 +1128,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="16"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -1147,8 +1155,8 @@
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="9" t="s">
         <v>23</v>
       </c>
@@ -1162,7 +1170,7 @@
       <c r="K9" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="L9" s="7"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="8"/>
       <c r="O9" t="s">
         <v>58</v>
@@ -1202,7 +1210,7 @@
       <c r="H10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="17"/>
+      <c r="I10" s="16"/>
       <c r="J10" s="7"/>
       <c r="K10" s="6" t="s">
         <v>110</v>
@@ -1238,7 +1246,7 @@
       <c r="E11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="6" t="s">
         <v>20</v>
       </c>
@@ -1267,7 +1275,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="6" t="s">
         <v>77</v>
       </c>
@@ -1284,7 +1292,7 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="K12" s="16"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="O12" t="s">
@@ -1313,10 +1321,12 @@
       <c r="D13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="16"/>
       <c r="I13" s="9" t="s">
         <v>82</v>
       </c>
@@ -1365,10 +1375,10 @@
         <v>111</v>
       </c>
       <c r="I14" s="7"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="8"/>
+      <c r="M14" s="16"/>
       <c r="O14" t="s">
         <v>100</v>
       </c>
@@ -1401,7 +1411,7 @@
       <c r="F15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
@@ -1432,8 +1442,8 @@
       <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="9" t="s">
         <v>95</v>
       </c>
@@ -1451,7 +1461,7 @@
       <c r="K16" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="7"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="8"/>
       <c r="O16" t="s">
         <v>99</v>
@@ -1487,7 +1497,7 @@
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="17"/>
+      <c r="I17" s="16"/>
       <c r="J17" s="6" t="s">
         <v>51</v>
       </c>
@@ -1523,8 +1533,10 @@
       <c r="E18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="H18" s="9" t="s">
         <v>49</v>
       </c>
@@ -1556,7 +1568,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="9" t="s">
         <v>32</v>
       </c>
@@ -1575,7 +1587,7 @@
       <c r="J19" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="K19" s="7"/>
+      <c r="K19" s="16"/>
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
       <c r="O19" t="s">
@@ -1604,12 +1616,12 @@
       <c r="D20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="6" t="s">
         <v>112</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="17"/>
+      <c r="H20" s="16"/>
       <c r="I20" s="7"/>
       <c r="J20" s="6" t="s">
         <v>58</v>
@@ -1658,10 +1670,10 @@
       <c r="I21" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="17"/>
+      <c r="J21" s="16"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
-      <c r="M21" s="8"/>
+      <c r="M21" s="16"/>
       <c r="O21" t="s">
         <v>15</v>
       </c>
@@ -1694,7 +1706,7 @@
       <c r="F22" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="17"/>
+      <c r="G22" s="16"/>
       <c r="H22" s="7"/>
       <c r="I22" s="9" t="s">
         <v>64</v>
@@ -1725,8 +1737,8 @@
       <c r="B23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="6" t="s">
         <v>103</v>
       </c>
@@ -1740,7 +1752,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="8"/>
       <c r="O23" t="s">
         <v>80</v>
@@ -1776,7 +1788,7 @@
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="17"/>
+      <c r="I24" s="16"/>
       <c r="J24" s="9" t="s">
         <v>90</v>
       </c>
@@ -1787,7 +1799,7 @@
         <v>12</v>
       </c>
       <c r="P24">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="R24" t="s">
         <v>68</v>
@@ -1810,7 +1822,7 @@
         <v>40</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="17"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="6" t="s">
@@ -1841,7 +1853,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="9" t="s">
         <v>68</v>
       </c>
@@ -1858,7 +1870,7 @@
       <c r="J26" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="7"/>
+      <c r="K26" s="16"/>
       <c r="L26" s="9" t="s">
         <v>70</v>
       </c>
@@ -1891,17 +1903,19 @@
       <c r="D27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="9" t="s">
         <v>92</v>
       </c>
       <c r="G27" s="7"/>
-      <c r="H27" s="17"/>
+      <c r="H27" s="16"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
+      <c r="M27" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="O27" t="s">
         <v>85</v>
       </c>
@@ -1939,12 +1953,10 @@
       <c r="I28" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="17"/>
+      <c r="J28" s="16"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="M28" s="16"/>
       <c r="O28" t="s">
         <v>51</v>
       </c>
@@ -1977,7 +1989,7 @@
       <c r="F29" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="6" t="s">
@@ -2008,8 +2020,8 @@
       <c r="B30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
       <c r="E30" s="9" t="s">
         <v>98</v>
       </c>
@@ -2023,7 +2035,7 @@
       <c r="K30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L30" s="7"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="11" t="s">
         <v>29</v>
       </c>
@@ -2047,7 +2059,7 @@
       <c r="B31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="17"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="9" t="s">
         <v>26</v>
       </c>
@@ -2061,7 +2073,7 @@
       <c r="H31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I31" s="17"/>
+      <c r="I31" s="16"/>
       <c r="J31" s="9" t="s">
         <v>89</v>
       </c>
@@ -2090,21 +2102,21 @@
       <c r="B32" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="21" t="s">
+      <c r="J32" s="17"/>
+      <c r="K32" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="L32" s="18"/>
-      <c r="M32" s="16"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="22"/>
       <c r="O32" t="s">
         <v>44</v>
       </c>
@@ -2247,7 +2259,7 @@
     <row r="42" spans="15:19" x14ac:dyDescent="0.35">
       <c r="P42">
         <f>SUM(P2:P41)</f>
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="R42" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
add a shitton of new constructors
</commit_message>
<xml_diff>
--- a/constructors.xlsx
+++ b/constructors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="143">
   <si>
     <t>Jan</t>
   </si>
@@ -411,16 +411,64 @@
   </si>
   <si>
     <t>QUIN ABARR</t>
+  </si>
+  <si>
+    <t>JACK JOSHI</t>
+  </si>
+  <si>
+    <t>LARRY AARONSON</t>
+  </si>
+  <si>
+    <t>MATTHEW HODGE</t>
+  </si>
+  <si>
+    <t>SONALEE RAU</t>
+  </si>
+  <si>
+    <t>JESS SHULMAN</t>
+  </si>
+  <si>
+    <t>BEN SHINDEL</t>
+  </si>
+  <si>
+    <t>JEREMY KOENIG</t>
+  </si>
+  <si>
+    <t>FINN VIGELAND</t>
+  </si>
+  <si>
+    <t>IAN RATHKEY</t>
+  </si>
+  <si>
+    <t>JOHN O'LEARY</t>
+  </si>
+  <si>
+    <t>PETER GORDON</t>
+  </si>
+  <si>
+    <t>RICHARD ALLEN</t>
+  </si>
+  <si>
+    <t>JAMES LARKIN</t>
+  </si>
+  <si>
+    <t>ANDREW PERICAK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -558,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -585,6 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W73"/>
+  <dimension ref="A1:W86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,7 +1006,7 @@
         <v>29</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -982,7 +1031,9 @@
       <c r="G3" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="26" t="s">
+        <v>130</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="2"/>
       <c r="K3" s="3" t="s">
@@ -1023,7 +1074,9 @@
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="26" t="s">
+        <v>131</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>78</v>
       </c>
@@ -1128,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -1169,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -1198,7 +1251,9 @@
       <c r="H8" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1210,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="R8" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -1249,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="R9" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S9">
         <v>1</v>
@@ -1288,13 +1343,13 @@
       <c r="L10" s="2"/>
       <c r="M10" s="15"/>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="P10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="S10">
         <v>1</v>
@@ -1331,13 +1386,13 @@
       <c r="L11" s="2"/>
       <c r="M11" s="15"/>
       <c r="O11" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="P11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="S11">
         <v>1</v>
@@ -1360,7 +1415,9 @@
       <c r="F12" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="1" t="s">
+        <v>133</v>
+      </c>
       <c r="H12" s="3" t="s">
         <v>96</v>
       </c>
@@ -1370,16 +1427,16 @@
       <c r="L12" s="2"/>
       <c r="M12" s="15"/>
       <c r="O12" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="P12">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="S12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
@@ -1415,16 +1472,16 @@
       </c>
       <c r="M13" s="15"/>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="P13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="S13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
@@ -1443,7 +1500,9 @@
       <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
         <v>110</v>
@@ -1454,16 +1513,16 @@
       <c r="L14" s="2"/>
       <c r="M14" s="16"/>
       <c r="O14" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="P14">
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="S14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
@@ -1497,16 +1556,16 @@
         <v>26</v>
       </c>
       <c r="O15" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="P15">
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
@@ -1521,7 +1580,9 @@
       <c r="E16" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="G16" s="3" t="s">
         <v>107</v>
       </c>
@@ -1540,16 +1601,16 @@
       <c r="L16" s="4"/>
       <c r="M16" s="15"/>
       <c r="O16" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="S16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.35">
@@ -1572,25 +1633,31 @@
         <v>47</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="H17" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="1" t="s">
         <v>50</v>
       </c>
       <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="15"/>
+      <c r="L17" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>140</v>
+      </c>
       <c r="O17" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="P17">
         <v>1</v>
       </c>
       <c r="R17" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.35">
@@ -1628,13 +1695,13 @@
         <v>32</v>
       </c>
       <c r="O18" t="s">
-        <v>117</v>
+        <v>31</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R18" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="S18">
         <v>1</v>
@@ -1654,8 +1721,12 @@
       <c r="E19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="F19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="H19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1667,13 +1738,13 @@
       <c r="L19" s="2"/>
       <c r="M19" s="15"/>
       <c r="O19" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="P19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R19" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="S19">
         <v>1</v>
@@ -1698,7 +1769,9 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>57</v>
       </c>
@@ -1710,13 +1783,13 @@
         <v>113</v>
       </c>
       <c r="O20" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="P20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R20" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="S20">
         <v>1</v>
@@ -1749,7 +1822,9 @@
         <v>75</v>
       </c>
       <c r="J21" s="4"/>
-      <c r="K21" s="2"/>
+      <c r="K21" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="L21" s="2"/>
       <c r="M21" s="16"/>
       <c r="O21" t="s">
@@ -1759,10 +1834,10 @@
         <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="S21">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.35">
@@ -1802,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="R22" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="S22">
         <v>1</v>
@@ -1820,7 +1895,9 @@
       <c r="E23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="G23" s="1" t="s">
         <v>98</v>
       </c>
@@ -1841,10 +1918,10 @@
         <v>1</v>
       </c>
       <c r="R23" t="s">
-        <v>124</v>
+        <v>34</v>
       </c>
       <c r="S23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.35">
@@ -1886,10 +1963,10 @@
         <v>3</v>
       </c>
       <c r="R24" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="S24">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.35">
@@ -1931,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="R25" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="S25">
         <v>1</v>
@@ -1951,7 +2028,9 @@
       <c r="E26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1972,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="R26" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="S26">
         <v>1</v>
@@ -2013,7 +2092,7 @@
         <v>2</v>
       </c>
       <c r="R27" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="S27">
         <v>2</v>
@@ -2035,7 +2114,9 @@
       <c r="E28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>33</v>
       </c>
@@ -2054,7 +2135,7 @@
         <v>20</v>
       </c>
       <c r="R28" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="S28">
         <v>1</v>
@@ -2074,7 +2155,7 @@
         <v>93</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>66</v>
@@ -2097,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="R29" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="S29">
         <v>1</v>
@@ -2139,10 +2220,10 @@
         <v>1</v>
       </c>
       <c r="R30" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="S30">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2184,10 +2265,10 @@
         <v>1</v>
       </c>
       <c r="R31" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="S31">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2219,7 +2300,7 @@
         <v>3</v>
       </c>
       <c r="R32" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="S32">
         <v>1</v>
@@ -2233,7 +2314,7 @@
         <v>1</v>
       </c>
       <c r="R33" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="S33">
         <v>1</v>
@@ -2247,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="R34" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="S34">
         <v>1</v>
@@ -2261,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="R35" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="S35">
         <v>1</v>
@@ -2275,10 +2356,10 @@
         <v>2</v>
       </c>
       <c r="R36" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="S36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="15:19" x14ac:dyDescent="0.35">
@@ -2289,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="R37" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="S37">
         <v>1</v>
@@ -2303,7 +2384,7 @@
         <v>1</v>
       </c>
       <c r="R38" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="S38">
         <v>1</v>
@@ -2317,10 +2398,10 @@
         <v>5</v>
       </c>
       <c r="R39" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="S39">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="15:19" x14ac:dyDescent="0.35">
@@ -2331,10 +2412,10 @@
         <v>2</v>
       </c>
       <c r="R40" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="S40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="15:19" x14ac:dyDescent="0.35">
@@ -2345,10 +2426,10 @@
         <v>1</v>
       </c>
       <c r="R41" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="S41">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="15:19" x14ac:dyDescent="0.35">
@@ -2359,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="R42" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="S42">
         <v>1</v>
@@ -2367,16 +2448,16 @@
     </row>
     <row r="43" spans="15:19" x14ac:dyDescent="0.35">
       <c r="O43" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="P43">
         <v>2</v>
       </c>
       <c r="R43" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="S43">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="15:19" x14ac:dyDescent="0.35">
@@ -2387,7 +2468,7 @@
         <v>3</v>
       </c>
       <c r="R44" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="S44">
         <v>1</v>
@@ -2401,10 +2482,10 @@
         <v>1</v>
       </c>
       <c r="R45" t="s">
-        <v>21</v>
+        <v>131</v>
       </c>
       <c r="S45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="15:19" x14ac:dyDescent="0.35">
@@ -2415,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="R46" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="S46">
         <v>1</v>
@@ -2427,15 +2508,15 @@
         <v>91</v>
       </c>
       <c r="R47" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="S47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="15:19" x14ac:dyDescent="0.35">
       <c r="R48" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="S48">
         <v>1</v>
@@ -2443,23 +2524,23 @@
     </row>
     <row r="49" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R49" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="S49">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R50" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="S50">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R51" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="S51">
         <v>1</v>
@@ -2467,31 +2548,31 @@
     </row>
     <row r="52" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R52" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="S52">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R53" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="S53">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R54" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="S54">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R55" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="S55">
         <v>1</v>
@@ -2499,7 +2580,7 @@
     </row>
     <row r="56" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R56" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="S56">
         <v>1</v>
@@ -2507,7 +2588,7 @@
     </row>
     <row r="57" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R57" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="S57">
         <v>1</v>
@@ -2515,15 +2596,15 @@
     </row>
     <row r="58" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R58" t="s">
-        <v>122</v>
+        <v>47</v>
       </c>
       <c r="S58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R59" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="S59">
         <v>1</v>
@@ -2531,15 +2612,15 @@
     </row>
     <row r="60" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R60" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="S60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R61" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="S61">
         <v>1</v>
@@ -2547,7 +2628,7 @@
     </row>
     <row r="62" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R62" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="S62">
         <v>1</v>
@@ -2555,23 +2636,23 @@
     </row>
     <row r="63" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R63" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="S63">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R64" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="S64">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R65" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="S65">
         <v>1</v>
@@ -2579,7 +2660,7 @@
     </row>
     <row r="66" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R66" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="S66">
         <v>1</v>
@@ -2587,7 +2668,7 @@
     </row>
     <row r="67" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R67" t="s">
-        <v>58</v>
+        <v>139</v>
       </c>
       <c r="S67">
         <v>1</v>
@@ -2595,7 +2676,7 @@
     </row>
     <row r="68" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R68" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="S68">
         <v>1</v>
@@ -2603,7 +2684,7 @@
     </row>
     <row r="69" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R69" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="S69">
         <v>1</v>
@@ -2611,15 +2692,15 @@
     </row>
     <row r="70" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R70" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="S70">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R71" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="S71">
         <v>1</v>
@@ -2627,16 +2708,120 @@
     </row>
     <row r="72" spans="18:19" x14ac:dyDescent="0.35">
       <c r="R72" t="s">
+        <v>104</v>
+      </c>
+      <c r="S72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R73" t="s">
+        <v>66</v>
+      </c>
+      <c r="S73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R74" t="s">
+        <v>69</v>
+      </c>
+      <c r="S74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R75" t="s">
+        <v>118</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R76" t="s">
+        <v>26</v>
+      </c>
+      <c r="S76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R77" t="s">
+        <v>35</v>
+      </c>
+      <c r="S77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R78" t="s">
+        <v>24</v>
+      </c>
+      <c r="S78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R79" t="s">
+        <v>62</v>
+      </c>
+      <c r="S79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R80" t="s">
+        <v>58</v>
+      </c>
+      <c r="S80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R81" t="s">
+        <v>114</v>
+      </c>
+      <c r="S81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R82" t="s">
+        <v>115</v>
+      </c>
+      <c r="S82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R83" t="s">
+        <v>88</v>
+      </c>
+      <c r="S83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R84" t="s">
+        <v>127</v>
+      </c>
+      <c r="S84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="R85" t="s">
         <v>14</v>
       </c>
-      <c r="S72">
+      <c r="S85">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="18:19" x14ac:dyDescent="0.35">
-      <c r="S73">
-        <f>SUM(S2:S72)</f>
-        <v>105</v>
+    <row r="86" spans="18:19" x14ac:dyDescent="0.35">
+      <c r="S86">
+        <f>SUM(S2:S85)</f>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>